<commit_message>
Termin mit Projektpartner & Zeiterfassung
</commit_message>
<xml_diff>
--- a/Zeiterfassung/Zeiterfassung_Gesamt.xlsx
+++ b/Zeiterfassung/Zeiterfassung_Gesamt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Samardzic\Documents\GitHub\PS_InfoEng\Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7297A28F-02F1-4121-8861-4CACECD38AC2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8B049EC8-64D1-406A-AE56-5293173F0AE4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
   <si>
     <t xml:space="preserve">Dusanic </t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Präsentation Erstellung für 1 Meileinstein &amp; Vorbereiten &amp; Projektplan erstellen</t>
+  </si>
+  <si>
+    <t>Abstimmung mit Projektpartner bzgl. Erhebungsinstrumen (Microsoft Forms)</t>
+  </si>
+  <si>
+    <t>Präsentation Erstellung für Meeting mit Projektpartner &amp; Vorbereiten</t>
   </si>
 </sst>
 </file>
@@ -968,7 +974,7 @@
                 <c:formatCode>_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11.5</c:v>
@@ -2126,7 +2132,7 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>Samardzic!F58</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <f>Dusanic!F58</f>
@@ -2262,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,53 +2460,93 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="B15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="20">
+        <v>43403</v>
+      </c>
+      <c r="D15" s="21">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E15" s="21">
+        <v>0.375</v>
+      </c>
       <c r="F15">
         <f>(Tabelle3[[#This Row],[bis]]*24)-(Tabelle3[[#This Row],[von]]*24)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="20">
+        <v>43403</v>
+      </c>
+      <c r="D16" s="21">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E16" s="21">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="F16">
         <f>(Tabelle3[[#This Row],[bis]]*24)-(Tabelle3[[#This Row],[von]]*24)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="20">
+        <v>43410</v>
+      </c>
+      <c r="D17" s="21">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="F17">
         <f>(Tabelle3[[#This Row],[bis]]*24)-(Tabelle3[[#This Row],[von]]*24)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="B18" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="20">
+        <v>43412</v>
+      </c>
+      <c r="D18" s="21">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E18" s="21">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="F18">
         <f>(Tabelle3[[#This Row],[bis]]*24)-(Tabelle3[[#This Row],[von]]*24)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="20">
+        <v>43415</v>
+      </c>
+      <c r="D19" s="21">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E19" s="21">
+        <v>0.875</v>
+      </c>
       <c r="F19">
         <f>(Tabelle3[[#This Row],[bis]]*24)-(Tabelle3[[#This Row],[von]]*24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -2892,7 +2938,7 @@
       <c r="E58" s="28"/>
       <c r="F58">
         <f>SUM(F7:F57)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>